<commit_message>
update pcb files hopefully for the last time
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="BOM_Board1_1_PCB_2025-10-14" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="BOM_Board1_1_PCB_2025-10-15" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>No.</t>
   </si>
@@ -91,16 +91,19 @@
     <t>3</t>
   </si>
   <si>
-    <t>J-S1206B4SW3-G2-A8</t>
-  </si>
-  <si>
-    <t>LED1</t>
-  </si>
-  <si>
-    <t>LED1206-RD</t>
-  </si>
-  <si>
-    <t>C2917491</t>
+    <t>YLED1206R</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>LED1206-FD</t>
+  </si>
+  <si>
+    <t>YONGYUTAI(永裕泰)</t>
+  </si>
+  <si>
+    <t>C28310439</t>
   </si>
   <si>
     <t>4</t>
@@ -680,10 +683,10 @@
         <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -691,31 +694,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -723,31 +726,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
@@ -755,31 +758,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
         <v>17</v>
@@ -787,31 +790,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J8" t="s">
         <v>17</v>

</xml_diff>